<commit_message>
Updated the .xlsx file
</commit_message>
<xml_diff>
--- a/Trabalho_calc_numerico.xlsx
+++ b/Trabalho_calc_numerico.xlsx
@@ -4,30 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Questao_01" sheetId="2" r:id="rId2"/>
-    <sheet name="Questao_02" sheetId="3" r:id="rId3"/>
-    <sheet name="Questao_03" sheetId="4" r:id="rId4"/>
+    <sheet name="Questao_01" sheetId="2" r:id="rId1"/>
+    <sheet name="Questao_02" sheetId="3" r:id="rId2"/>
+    <sheet name="Questao_03" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211" fullPrecision="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="27">
-  <si>
-    <t>Questão</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
   <si>
     <t>Intervalo</t>
   </si>
   <si>
-    <t>Raiz aproximada</t>
-  </si>
-  <si>
     <t>[-2; -1.5]</t>
   </si>
   <si>
@@ -35,12 +28,6 @@
   </si>
   <si>
     <t>Iterações</t>
-  </si>
-  <si>
-    <t>Método de refinamento</t>
-  </si>
-  <si>
-    <t>Bissecção</t>
   </si>
   <si>
     <t>Tempo gasto (s)</t>
@@ -171,13 +158,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -239,7 +226,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="14" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A2:E10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -248,18 +235,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Método " dataDxfId="20"/>
-    <tableColumn id="2" name="Intervalo" dataDxfId="19"/>
-    <tableColumn id="3" name="Tempo gasto (s)" dataDxfId="18"/>
-    <tableColumn id="4" name="Raiz Aproximada" dataDxfId="17"/>
-    <tableColumn id="5" name="Iterações" dataDxfId="16"/>
+    <tableColumn id="1" name="Método " dataDxfId="18"/>
+    <tableColumn id="2" name="Intervalo" dataDxfId="17"/>
+    <tableColumn id="3" name="Tempo gasto (s)" dataDxfId="16"/>
+    <tableColumn id="4" name="Raiz Aproximada" dataDxfId="15"/>
+    <tableColumn id="5" name="Iterações" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A2:E10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A2:E10" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A2:E10">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -268,18 +255,18 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Método " dataDxfId="13"/>
-    <tableColumn id="2" name="Intervalo" dataDxfId="12"/>
-    <tableColumn id="3" name="Tempo gasto (s)" dataDxfId="11"/>
-    <tableColumn id="4" name="Raiz Aproximada" dataDxfId="10"/>
-    <tableColumn id="5" name="Iterações" dataDxfId="9"/>
+    <tableColumn id="1" name="Método " dataDxfId="11"/>
+    <tableColumn id="2" name="Intervalo" dataDxfId="10"/>
+    <tableColumn id="3" name="Tempo gasto (s)" dataDxfId="9"/>
+    <tableColumn id="4" name="Raiz Aproximada" dataDxfId="8"/>
+    <tableColumn id="5" name="Iterações" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A2:E14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A2:E14" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A2:E14">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -288,11 +275,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Método " dataDxfId="6"/>
-    <tableColumn id="2" name="Intervalo" dataDxfId="5"/>
-    <tableColumn id="3" name="Tempo gasto (s)" dataDxfId="4"/>
-    <tableColumn id="4" name="Raiz Aproximada" dataDxfId="3"/>
-    <tableColumn id="5" name="Iterações" dataDxfId="2"/>
+    <tableColumn id="1" name="Método " dataDxfId="4"/>
+    <tableColumn id="2" name="Intervalo" dataDxfId="3"/>
+    <tableColumn id="3" name="Tempo gasto (s)" dataDxfId="2"/>
+    <tableColumn id="4" name="Raiz Aproximada" dataDxfId="1"/>
+    <tableColumn id="5" name="Iterações" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -585,296 +572,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-4.7033199999999997</v>
-      </c>
-      <c r="E2" s="1">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-1.7416400000000001</v>
-      </c>
-      <c r="E3" s="1">
-        <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-1.2737099999999999</v>
-      </c>
-      <c r="E4" s="1">
-        <v>12</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1.14558</v>
-      </c>
-      <c r="E5" s="1">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-4.7133900000000004</v>
-      </c>
-      <c r="E6" s="1">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-1.54715</v>
-      </c>
-      <c r="E7" s="1">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.19496</v>
-      </c>
-      <c r="E8" s="1">
-        <v>13</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -888,7 +588,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -897,30 +597,30 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>-4.7033199999999997</v>
@@ -931,13 +631,13 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
         <v>-1.7416400000000001</v>
@@ -948,13 +648,13 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" s="1">
         <v>-4.7033199999999997</v>
@@ -965,13 +665,13 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <v>-1.74614</v>
@@ -982,13 +682,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3">
         <v>-4.7033199999999997</v>
@@ -999,13 +699,13 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D8" s="1">
         <v>-1.74613</v>
@@ -1016,13 +716,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1">
         <v>-4.7033199999999997</v>
@@ -1033,13 +733,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1">
         <v>-1.74613</v>
@@ -1132,7 +832,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -1151,7 +851,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1160,30 +860,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>-1.2737099999999999</v>
@@ -1194,13 +894,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5">
         <v>1.14558</v>
@@ -1211,13 +911,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5">
         <v>-1.2737099999999999</v>
@@ -1228,13 +928,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5">
         <v>1.14558</v>
@@ -1245,13 +945,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2">
         <v>-1.2737099999999999</v>
@@ -1262,13 +962,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5">
         <v>1.14557</v>
@@ -1279,13 +979,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D9" s="5">
         <v>-1.2737099999999999</v>
@@ -1296,13 +996,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D10" s="5">
         <v>1.14557</v>
@@ -1322,11 +1022,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="A1:E14"/>
     </sheetView>
   </sheetViews>
@@ -1341,7 +1041,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1350,30 +1050,30 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1">
         <v>-4.7133900000000004</v>
@@ -1384,13 +1084,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>-1.54715</v>
@@ -1401,13 +1101,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <v>1.19496</v>
@@ -1418,13 +1118,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1">
         <v>-4.7133900000000004</v>
@@ -1435,13 +1135,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D7" s="1">
         <v>-1.54714</v>
@@ -1452,13 +1152,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1">
         <v>1.19496</v>
@@ -1469,13 +1169,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3">
         <v>-4.7133799999999999</v>
@@ -1486,13 +1186,13 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
         <v>-1.54714</v>
@@ -1503,13 +1203,13 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3">
         <v>1.19496</v>
@@ -1520,13 +1220,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D12" s="4">
         <v>-4.7133799999999999</v>
@@ -1537,13 +1237,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4">
         <v>-1.54714</v>
@@ -1554,13 +1254,13 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4">
         <v>1.19496</v>

</xml_diff>